<commit_message>
Updated README and Agile document
</commit_message>
<xml_diff>
--- a/Agile_Document.xlsx
+++ b/Agile_Document.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\github project\agent-orchestration-langchain\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB650FCE-A96F-457D-B715-7A100B38936A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Product Backlog" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sprint Backlog" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Stand up Meeting" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Retrospection" sheetId="4" r:id="rId7"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Stand up Meeting" sheetId="3" r:id="rId3"/>
+    <sheet name="Retrospection" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -112,9 +121,6 @@
     <t>US006</t>
   </si>
   <si>
-    <t>As a developer, I want to design a workflow using REST API so that external system can trigger it.</t>
-  </si>
-  <si>
     <t>Orchestration Logic</t>
   </si>
   <si>
@@ -128,9 +134,6 @@
   </si>
   <si>
     <t>Could Have</t>
-  </si>
-  <si>
-    <t>REST API</t>
   </si>
   <si>
     <t>Frontend Team</t>
@@ -450,67 +453,81 @@
   </si>
   <si>
     <t>Created separate agents with clearly defined responsibilities</t>
+  </si>
+  <si>
+    <t>As a developer, I want to design a workflow using FAST API so that external system can trigger it.</t>
+  </si>
+  <si>
+    <t>FAST API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m-d-yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm-dd-yyyy"/>
-    <numFmt numFmtId="166" formatCode="d mmm"/>
+    <numFmt numFmtId="164" formatCode="m\-d\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm\-dd\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="d\ mmm"/>
   </numFmts>
   <fonts count="11">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times Roman&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
     </font>
@@ -520,7 +537,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -554,7 +571,13 @@
     </fill>
   </fills>
   <borders count="8">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -568,14 +591,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -587,8 +614,11 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -598,11 +628,16 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -611,142 +646,118 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -936,27 +947,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.5"/>
-    <col customWidth="1" min="2" max="3" width="9.75"/>
-    <col customWidth="1" min="4" max="4" width="108.38"/>
-    <col customWidth="1" min="5" max="5" width="14.63"/>
-    <col customWidth="1" min="6" max="6" width="28.63"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="108.36328125" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="28.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.0" customHeight="1">
+    <row r="1" spans="1:8" ht="27" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="12.5">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1008,7 +1024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="12.5">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1034,7 +1050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="12.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1076,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="12.5">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1086,7 +1102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="12.5">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1112,7 +1128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="12.5">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1123,22 +1139,22 @@
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>143</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.5">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1146,949 +1162,952 @@
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="58.75"/>
-    <col customWidth="1" min="5" max="5" width="15.25"/>
-    <col customWidth="1" min="6" max="6" width="13.88"/>
-    <col customWidth="1" min="7" max="7" width="27.38"/>
-    <col customWidth="1" min="8" max="8" width="11.5"/>
-    <col customWidth="1" min="9" max="9" width="22.75"/>
+    <col min="3" max="3" width="58.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="27.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.75" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" ht="33.75" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="T1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="U1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="V1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:23" ht="23.25" customHeight="1">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="6">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.5">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" ht="23.25" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10">
-        <v>42.0</v>
-      </c>
-      <c r="J2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="K2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="L2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="M2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="N2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="O2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="P2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="R2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="S2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="T2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="U2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="V2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="W2" s="10">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" ht="15.5">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="C4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" spans="1:23" ht="14">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>76</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="7">
+        <v>6</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.5">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="11" t="s">
+      <c r="C6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="7">
+        <v>7</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:23" ht="15.5">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="11">
-        <v>7.0</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="17">
-        <v>45700.0</v>
+      <c r="E7" s="12">
+        <v>45700</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" ht="15.5">
+      <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="D8" s="12">
+        <v>45942</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="17">
-        <v>45942.0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="7">
+        <v>10</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" ht="15.5">
+      <c r="A9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="11">
-        <v>10.0</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="D9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="7">
+        <v>8</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="12.5">
+      <c r="A10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" s="11">
-        <v>8.0</v>
-      </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="S9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="U9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="V9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="W9" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" ht="12.5">
+      <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="11" t="s">
+      <c r="C11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="D11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="13">
+        <v>46174</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="19">
-        <v>46174.0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.0"/>
-    <col customWidth="1" min="2" max="2" width="14.25"/>
-    <col customWidth="1" min="3" max="3" width="40.75"/>
-    <col customWidth="1" min="4" max="4" width="37.5"/>
-    <col customWidth="1" min="6" max="6" width="13.88"/>
-    <col customWidth="1" min="7" max="7" width="14.38"/>
-    <col customWidth="1" min="8" max="8" width="14.0"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="12.5">
+      <c r="A2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="12.5">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.5">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12.5">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="12.5">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="12.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="15.0"/>
-    <col customWidth="1" min="4" max="4" width="13.63"/>
-    <col customWidth="1" min="5" max="5" width="18.38"/>
-    <col customWidth="1" min="6" max="6" width="50.88"/>
-    <col customWidth="1" min="7" max="7" width="46.63"/>
-    <col customWidth="1" min="8" max="8" width="41.5"/>
-    <col customWidth="1" min="9" max="9" width="47.75"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" customWidth="1"/>
+    <col min="6" max="6" width="50.90625" customWidth="1"/>
+    <col min="7" max="7" width="46.6328125" customWidth="1"/>
+    <col min="8" max="8" width="41.453125" customWidth="1"/>
+    <col min="9" max="9" width="47.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24.0" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="24" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="E1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="I1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="22" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="12.5">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18">
+        <v>45973</v>
+      </c>
+      <c r="D2" s="18">
+        <v>45986</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="24">
-        <v>45973.0</v>
-      </c>
-      <c r="D2" s="24">
-        <v>45986.0</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="G2" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="H2" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="I2" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="25" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="12.5">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="18">
+        <v>45987</v>
+      </c>
+      <c r="D3" s="18">
+        <v>46000</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="24">
-        <v>45987.0</v>
-      </c>
-      <c r="D3" s="24">
-        <v>46000.0</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="26" t="s">
+      <c r="H3" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="I3" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="25" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="12.5">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="18">
+        <v>46001</v>
+      </c>
+      <c r="D4" s="18">
+        <v>46014</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="G4" s="22" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="24">
-        <v>46001.0</v>
-      </c>
-      <c r="D4" s="24">
-        <v>46014.0</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="26" t="s">
+      <c r="H4" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="I4" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="29"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="33"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.5">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.5">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.5">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.5">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>